<commit_message>
Change GAM value for N-lim from 276.37 to 154.94
</commit_message>
<xml_diff>
--- a/supplementary_files/Supplementary Materials 2.xlsx
+++ b/supplementary_files/Supplementary Materials 2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hvdin\Desktop\rt_manuscript_supplements\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A70FFA92-D074-473C-8BC4-A140F129FA0C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCE7D160-B7FD-4A30-A057-8A469BC98461}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="984" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="984" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="NOTES" sheetId="5" r:id="rId1"/>
@@ -14839,9 +14839,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -14849,6 +14846,9 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -15235,7 +15235,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53DB90C0-3C5F-484E-B678-15283E933469}">
   <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
   <cols>
@@ -15367,7 +15367,7 @@
       </c>
     </row>
     <row r="2" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="23" t="s">
         <v>4682</v>
       </c>
       <c r="B2" s="12" t="s">
@@ -15376,7 +15376,7 @@
       <c r="C2" s="12"/>
     </row>
     <row r="3" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="25"/>
+      <c r="A3" s="24"/>
       <c r="B3" s="13" t="s">
         <v>4684</v>
       </c>
@@ -15396,9 +15396,9 @@
       </c>
     </row>
     <row r="5" spans="1:3" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="23"/>
-      <c r="B5" s="23"/>
-      <c r="C5" s="22"/>
+      <c r="A5" s="22"/>
+      <c r="B5" s="22"/>
+      <c r="C5" s="25"/>
     </row>
     <row r="6" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="21" t="s">
@@ -15407,12 +15407,12 @@
       <c r="B6" s="21" t="s">
         <v>4690</v>
       </c>
-      <c r="C6" s="22"/>
+      <c r="C6" s="25"/>
     </row>
     <row r="7" spans="1:3" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="23"/>
-      <c r="B7" s="23"/>
-      <c r="C7" s="22"/>
+      <c r="A7" s="22"/>
+      <c r="B7" s="22"/>
+      <c r="C7" s="25"/>
     </row>
     <row r="8" spans="1:3" ht="48.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="21" t="s">
@@ -15421,12 +15421,12 @@
       <c r="B8" s="21" t="s">
         <v>4692</v>
       </c>
-      <c r="C8" s="22"/>
+      <c r="C8" s="25"/>
     </row>
     <row r="9" spans="1:3" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="23"/>
-      <c r="B9" s="23"/>
-      <c r="C9" s="23"/>
+      <c r="A9" s="22"/>
+      <c r="B9" s="22"/>
+      <c r="C9" s="22"/>
     </row>
     <row r="10" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="21" t="s">
@@ -15440,9 +15440,9 @@
       </c>
     </row>
     <row r="11" spans="1:3" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="23"/>
-      <c r="B11" s="23"/>
-      <c r="C11" s="23"/>
+      <c r="A11" s="22"/>
+      <c r="B11" s="22"/>
+      <c r="C11" s="22"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="21" t="s">
@@ -15456,9 +15456,9 @@
       </c>
     </row>
     <row r="13" spans="1:3" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="23"/>
-      <c r="B13" s="23"/>
-      <c r="C13" s="23"/>
+      <c r="A13" s="22"/>
+      <c r="B13" s="22"/>
+      <c r="C13" s="22"/>
     </row>
     <row r="14" spans="1:3" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="21" t="s">
@@ -15472,9 +15472,9 @@
       </c>
     </row>
     <row r="15" spans="1:3" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="23"/>
-      <c r="B15" s="23"/>
-      <c r="C15" s="23"/>
+      <c r="A15" s="22"/>
+      <c r="B15" s="22"/>
+      <c r="C15" s="22"/>
     </row>
     <row r="16" spans="1:3" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="21" t="s">
@@ -15488,9 +15488,9 @@
       </c>
     </row>
     <row r="17" spans="1:3" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="23"/>
-      <c r="B17" s="23"/>
-      <c r="C17" s="23"/>
+      <c r="A17" s="22"/>
+      <c r="B17" s="22"/>
+      <c r="C17" s="22"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="21" t="s">
@@ -15504,9 +15504,9 @@
       </c>
     </row>
     <row r="19" spans="1:3" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="23"/>
-      <c r="B19" s="23"/>
-      <c r="C19" s="23"/>
+      <c r="A19" s="22"/>
+      <c r="B19" s="22"/>
+      <c r="C19" s="22"/>
     </row>
     <row r="20" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="15" t="s">
@@ -15529,15 +15529,15 @@
       </c>
     </row>
     <row r="22" spans="1:3" ht="31.2" x14ac:dyDescent="0.25">
-      <c r="A22" s="22"/>
-      <c r="B22" s="22"/>
+      <c r="A22" s="25"/>
+      <c r="B22" s="25"/>
       <c r="C22" s="14" t="s">
         <v>4713</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="23"/>
-      <c r="B23" s="23"/>
+      <c r="A23" s="22"/>
+      <c r="B23" s="22"/>
       <c r="C23" s="13"/>
     </row>
     <row r="24" spans="1:3" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
@@ -15552,9 +15552,9 @@
       </c>
     </row>
     <row r="25" spans="1:3" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="23"/>
-      <c r="B25" s="23"/>
-      <c r="C25" s="23"/>
+      <c r="A25" s="22"/>
+      <c r="B25" s="22"/>
+      <c r="C25" s="22"/>
     </row>
     <row r="26" spans="1:3" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="21" t="s">
@@ -15568,9 +15568,9 @@
       </c>
     </row>
     <row r="27" spans="1:3" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="23"/>
-      <c r="B27" s="23"/>
-      <c r="C27" s="23"/>
+      <c r="A27" s="22"/>
+      <c r="B27" s="22"/>
+      <c r="C27" s="22"/>
     </row>
     <row r="28" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="15" t="s">
@@ -15585,43 +15585,43 @@
       <c r="A29" s="15" t="s">
         <v>4722</v>
       </c>
-      <c r="B29" s="22"/>
-      <c r="C29" s="22"/>
+      <c r="B29" s="25"/>
+      <c r="C29" s="25"/>
     </row>
     <row r="30" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="15" t="s">
         <v>4723</v>
       </c>
-      <c r="B30" s="22"/>
-      <c r="C30" s="22"/>
+      <c r="B30" s="25"/>
+      <c r="C30" s="25"/>
     </row>
     <row r="31" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="15" t="s">
         <v>4724</v>
       </c>
-      <c r="B31" s="22"/>
-      <c r="C31" s="22"/>
+      <c r="B31" s="25"/>
+      <c r="C31" s="25"/>
     </row>
     <row r="32" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="15" t="s">
         <v>4725</v>
       </c>
-      <c r="B32" s="22"/>
-      <c r="C32" s="22"/>
+      <c r="B32" s="25"/>
+      <c r="C32" s="25"/>
     </row>
     <row r="33" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="15" t="s">
         <v>4726</v>
       </c>
-      <c r="B33" s="22"/>
-      <c r="C33" s="22"/>
+      <c r="B33" s="25"/>
+      <c r="C33" s="25"/>
     </row>
     <row r="34" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="15" t="s">
         <v>4727</v>
       </c>
-      <c r="B34" s="23"/>
-      <c r="C34" s="23"/>
+      <c r="B34" s="22"/>
+      <c r="C34" s="22"/>
     </row>
     <row r="35" spans="1:3" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A35" s="16" t="s">
@@ -15634,7 +15634,7 @@
       </c>
     </row>
     <row r="39" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="24" t="s">
+      <c r="A39" s="23" t="s">
         <v>4682</v>
       </c>
       <c r="B39" s="12" t="s">
@@ -15643,7 +15643,7 @@
       <c r="C39" s="12"/>
     </row>
     <row r="40" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="25"/>
+      <c r="A40" s="24"/>
       <c r="B40" s="13" t="s">
         <v>4684</v>
       </c>
@@ -15663,9 +15663,9 @@
       </c>
     </row>
     <row r="42" spans="1:3" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="23"/>
-      <c r="B42" s="23"/>
-      <c r="C42" s="23"/>
+      <c r="A42" s="22"/>
+      <c r="B42" s="22"/>
+      <c r="C42" s="22"/>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="21" t="s">
@@ -15679,9 +15679,9 @@
       </c>
     </row>
     <row r="44" spans="1:3" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="23"/>
-      <c r="B44" s="23"/>
-      <c r="C44" s="23"/>
+      <c r="A44" s="22"/>
+      <c r="B44" s="22"/>
+      <c r="C44" s="22"/>
     </row>
     <row r="45" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="15" t="s">
@@ -15696,43 +15696,43 @@
       <c r="A46" s="15" t="s">
         <v>4739</v>
       </c>
-      <c r="B46" s="22"/>
-      <c r="C46" s="22"/>
+      <c r="B46" s="25"/>
+      <c r="C46" s="25"/>
     </row>
     <row r="47" spans="1:3" ht="31.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="15" t="s">
         <v>4740</v>
       </c>
-      <c r="B47" s="22"/>
-      <c r="C47" s="22"/>
+      <c r="B47" s="25"/>
+      <c r="C47" s="25"/>
     </row>
     <row r="48" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="15" t="s">
         <v>4741</v>
       </c>
-      <c r="B48" s="22"/>
-      <c r="C48" s="22"/>
+      <c r="B48" s="25"/>
+      <c r="C48" s="25"/>
     </row>
     <row r="49" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="15" t="s">
         <v>4742</v>
       </c>
-      <c r="B49" s="22"/>
-      <c r="C49" s="22"/>
+      <c r="B49" s="25"/>
+      <c r="C49" s="25"/>
     </row>
     <row r="50" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="15" t="s">
         <v>4743</v>
       </c>
-      <c r="B50" s="22"/>
-      <c r="C50" s="22"/>
+      <c r="B50" s="25"/>
+      <c r="C50" s="25"/>
     </row>
     <row r="51" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="15" t="s">
         <v>4744</v>
       </c>
-      <c r="B51" s="23"/>
-      <c r="C51" s="23"/>
+      <c r="B51" s="22"/>
+      <c r="C51" s="22"/>
     </row>
     <row r="52" spans="1:3" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A52" s="16" t="s">
@@ -15784,6 +15784,34 @@
     </row>
   </sheetData>
   <mergeCells count="42">
+    <mergeCell ref="B45:B51"/>
+    <mergeCell ref="C45:C51"/>
+    <mergeCell ref="A41:A42"/>
+    <mergeCell ref="B41:B42"/>
+    <mergeCell ref="C41:C42"/>
+    <mergeCell ref="A43:A44"/>
+    <mergeCell ref="B43:B44"/>
+    <mergeCell ref="C43:C44"/>
+    <mergeCell ref="A39:A40"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="A21:A23"/>
+    <mergeCell ref="B21:B23"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="A26:A27"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="B28:B34"/>
+    <mergeCell ref="C28:C34"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C9"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="B6:B7"/>
     <mergeCell ref="A16:A17"/>
     <mergeCell ref="B16:B17"/>
     <mergeCell ref="C16:C17"/>
@@ -15798,34 +15826,6 @@
     <mergeCell ref="A14:A15"/>
     <mergeCell ref="B14:B15"/>
     <mergeCell ref="C14:C15"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C9"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="A39:A40"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="A21:A23"/>
-    <mergeCell ref="B21:B23"/>
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="A26:A27"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="C26:C27"/>
-    <mergeCell ref="B28:B34"/>
-    <mergeCell ref="C28:C34"/>
-    <mergeCell ref="B45:B51"/>
-    <mergeCell ref="C45:C51"/>
-    <mergeCell ref="A41:A42"/>
-    <mergeCell ref="B41:B42"/>
-    <mergeCell ref="C41:C42"/>
-    <mergeCell ref="A43:A44"/>
-    <mergeCell ref="B43:B44"/>
-    <mergeCell ref="C43:C44"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -15836,7 +15836,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0111484F-11D4-4F10-BD6F-922F3BE2F87B}">
   <dimension ref="A1:K60"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
   <cols>
@@ -15934,7 +15936,7 @@
         <v>0.16</v>
       </c>
       <c r="E3" s="5">
-        <v>0.14000000000000001</v>
+        <v>0.17</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>2150</v>
@@ -16001,7 +16003,7 @@
         <v>0.12</v>
       </c>
       <c r="E5" s="5">
-        <v>6.6000000000000003E-2</v>
+        <v>0.08</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>2150</v>

</xml_diff>

<commit_message>
Change PDAGATpc/pe_rm to irreversible
</commit_message>
<xml_diff>
--- a/supplementary_files/Supplementary Materials 2.xlsx
+++ b/supplementary_files/Supplementary Materials 2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hvdin\Desktop\rt_manuscript_supplements\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hvdin\Desktop\rt_manuscript\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCE7D160-B7FD-4A30-A057-8A469BC98461}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44A21B78-A025-4230-BB3B-1BDD55E9E5E3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="984" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="746" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="NOTES" sheetId="5" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11218" uniqueCount="4809">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11243" uniqueCount="4834">
   <si>
     <t>gene_id</t>
   </si>
@@ -13580,12 +13580,6 @@
     <t>Fatty acid secretion KO</t>
   </si>
   <si>
-    <t>PDAGATpc_rm</t>
-  </si>
-  <si>
-    <t>PDAGATpe_rm</t>
-  </si>
-  <si>
     <t>TAGL_l</t>
   </si>
   <si>
@@ -13599,45 +13593,6 @@
   </si>
   <si>
     <t>DAGL_m</t>
-  </si>
-  <si>
-    <t>FACOA120tabc_x</t>
-  </si>
-  <si>
-    <t>FACOA140tabc_x</t>
-  </si>
-  <si>
-    <t>FACOA160tabc_x</t>
-  </si>
-  <si>
-    <t>FACOA161tabc_x</t>
-  </si>
-  <si>
-    <t>FACOA180tabc_x</t>
-  </si>
-  <si>
-    <t>FACOA181tabc_x</t>
-  </si>
-  <si>
-    <t>FACOA182tabc_x</t>
-  </si>
-  <si>
-    <t>FACOA183tabc_x</t>
-  </si>
-  <si>
-    <t>FACOA200tabc_x</t>
-  </si>
-  <si>
-    <t>FACOA220tabc_x</t>
-  </si>
-  <si>
-    <t>FACOA240tabc_x</t>
-  </si>
-  <si>
-    <t>FACOA260tabc_x</t>
-  </si>
-  <si>
-    <t>TTDCAt_c_x</t>
   </si>
   <si>
     <t>EX_hxa_e</t>
@@ -14628,6 +14583,126 @@
   </si>
   <si>
     <t>13C-MFA data from Wasylenko et al., 2015 (PMID: 25747307) for Y. lipolytica used in this study is also provided</t>
+  </si>
+  <si>
+    <t>ACOAO100_x</t>
+  </si>
+  <si>
+    <t>ACOAO120_x</t>
+  </si>
+  <si>
+    <t>ACOAO260_x</t>
+  </si>
+  <si>
+    <t>ACOAO160_x</t>
+  </si>
+  <si>
+    <t>ACOAO180_x</t>
+  </si>
+  <si>
+    <t>ACOAO140_x</t>
+  </si>
+  <si>
+    <t>ACOAO40_x</t>
+  </si>
+  <si>
+    <t>ACOAO60_x</t>
+  </si>
+  <si>
+    <t>ACOAO80_x</t>
+  </si>
+  <si>
+    <t>ACOAO200_x</t>
+  </si>
+  <si>
+    <t>ACOAO220_x</t>
+  </si>
+  <si>
+    <t>ACOAO240_x</t>
+  </si>
+  <si>
+    <t>ACOAO161b_x</t>
+  </si>
+  <si>
+    <t>ACOAO141b_x</t>
+  </si>
+  <si>
+    <t>ACOAO121a_x</t>
+  </si>
+  <si>
+    <t>ACOAO181a_x</t>
+  </si>
+  <si>
+    <t>ACOAO161a_x</t>
+  </si>
+  <si>
+    <t>ACOAO141a_x</t>
+  </si>
+  <si>
+    <t>ACOAO100_m</t>
+  </si>
+  <si>
+    <t>ACOAO120_m</t>
+  </si>
+  <si>
+    <t>ACOAO160_m</t>
+  </si>
+  <si>
+    <t>ACOAO180_m</t>
+  </si>
+  <si>
+    <t>ACOAO140_m</t>
+  </si>
+  <si>
+    <t>ACOAO40_m</t>
+  </si>
+  <si>
+    <t>ACOAO60_m</t>
+  </si>
+  <si>
+    <t>ACOAO80_m</t>
+  </si>
+  <si>
+    <t>ACOAO161b_m</t>
+  </si>
+  <si>
+    <t>ACOAO141b_m</t>
+  </si>
+  <si>
+    <t>ACOAO121a_m</t>
+  </si>
+  <si>
+    <t>ACOAO181a_m</t>
+  </si>
+  <si>
+    <t>ACOAO161a_m</t>
+  </si>
+  <si>
+    <t>ACOAO141a_m</t>
+  </si>
+  <si>
+    <t>ACOAD40f_m</t>
+  </si>
+  <si>
+    <t>ACOAD60f_m</t>
+  </si>
+  <si>
+    <t>ACOADm30f_m</t>
+  </si>
+  <si>
+    <t>ACOADm40f_m</t>
+  </si>
+  <si>
+    <t>ACOAD80f_m</t>
+  </si>
+  <si>
+    <t>ACOADm50f_m</t>
+  </si>
+  <si>
+    <t>FAOX182lump_x</t>
+  </si>
+  <si>
+    <t>FAOX183lump_x</t>
   </si>
 </sst>
 </file>
@@ -14839,6 +14914,9 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -14846,9 +14924,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -15251,7 +15326,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>4681</v>
+        <v>4666</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -15262,10 +15337,10 @@
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="2"/>
       <c r="B5" s="2" t="s">
-        <v>4745</v>
+        <v>4730</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>4746</v>
+        <v>4731</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -15327,18 +15402,18 @@
         <v>2395</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>4680</v>
+        <v>4665</v>
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B18" s="2"/>
       <c r="C18" s="3" t="s">
-        <v>4755</v>
+        <v>4740</v>
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.3">
       <c r="C19" s="3" t="s">
-        <v>4808</v>
+        <v>4793</v>
       </c>
     </row>
   </sheetData>
@@ -15363,420 +15438,420 @@
   <sheetData>
     <row r="1" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="17" t="s">
-        <v>4729</v>
+        <v>4714</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="23" t="s">
-        <v>4682</v>
+      <c r="A2" s="24" t="s">
+        <v>4667</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>4683</v>
+        <v>4668</v>
       </c>
       <c r="C2" s="12"/>
     </row>
     <row r="3" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="24"/>
+      <c r="A3" s="25"/>
       <c r="B3" s="13" t="s">
-        <v>4684</v>
+        <v>4669</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>4685</v>
+        <v>4670</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="48.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="21" t="s">
-        <v>4686</v>
+        <v>4671</v>
       </c>
       <c r="B4" s="21" t="s">
-        <v>4687</v>
+        <v>4672</v>
       </c>
       <c r="C4" s="21" t="s">
-        <v>4688</v>
+        <v>4673</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="22"/>
-      <c r="B5" s="22"/>
-      <c r="C5" s="25"/>
+      <c r="A5" s="23"/>
+      <c r="B5" s="23"/>
+      <c r="C5" s="22"/>
     </row>
     <row r="6" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="21" t="s">
-        <v>4689</v>
+        <v>4674</v>
       </c>
       <c r="B6" s="21" t="s">
-        <v>4690</v>
-      </c>
-      <c r="C6" s="25"/>
+        <v>4675</v>
+      </c>
+      <c r="C6" s="22"/>
     </row>
     <row r="7" spans="1:3" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="22"/>
-      <c r="B7" s="22"/>
-      <c r="C7" s="25"/>
+      <c r="A7" s="23"/>
+      <c r="B7" s="23"/>
+      <c r="C7" s="22"/>
     </row>
     <row r="8" spans="1:3" ht="48.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="21" t="s">
-        <v>4691</v>
+        <v>4676</v>
       </c>
       <c r="B8" s="21" t="s">
-        <v>4692</v>
-      </c>
-      <c r="C8" s="25"/>
+        <v>4677</v>
+      </c>
+      <c r="C8" s="22"/>
     </row>
     <row r="9" spans="1:3" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="22"/>
-      <c r="B9" s="22"/>
-      <c r="C9" s="22"/>
+      <c r="A9" s="23"/>
+      <c r="B9" s="23"/>
+      <c r="C9" s="23"/>
     </row>
     <row r="10" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="21" t="s">
-        <v>4693</v>
+        <v>4678</v>
       </c>
       <c r="B10" s="21" t="s">
-        <v>4694</v>
+        <v>4679</v>
       </c>
       <c r="C10" s="21" t="s">
-        <v>4695</v>
+        <v>4680</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="22"/>
-      <c r="B11" s="22"/>
-      <c r="C11" s="22"/>
+      <c r="A11" s="23"/>
+      <c r="B11" s="23"/>
+      <c r="C11" s="23"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="21" t="s">
-        <v>4696</v>
+        <v>4681</v>
       </c>
       <c r="B12" s="21" t="s">
-        <v>4697</v>
+        <v>4682</v>
       </c>
       <c r="C12" s="21" t="s">
-        <v>4698</v>
+        <v>4683</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="22"/>
-      <c r="B13" s="22"/>
-      <c r="C13" s="22"/>
+      <c r="A13" s="23"/>
+      <c r="B13" s="23"/>
+      <c r="C13" s="23"/>
     </row>
     <row r="14" spans="1:3" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="21" t="s">
-        <v>4699</v>
+        <v>4684</v>
       </c>
       <c r="B14" s="21" t="s">
-        <v>4700</v>
+        <v>4685</v>
       </c>
       <c r="C14" s="21" t="s">
-        <v>4701</v>
+        <v>4686</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="22"/>
-      <c r="B15" s="22"/>
-      <c r="C15" s="22"/>
+      <c r="A15" s="23"/>
+      <c r="B15" s="23"/>
+      <c r="C15" s="23"/>
     </row>
     <row r="16" spans="1:3" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="21" t="s">
-        <v>4702</v>
+        <v>4687</v>
       </c>
       <c r="B16" s="21" t="s">
-        <v>4703</v>
+        <v>4688</v>
       </c>
       <c r="C16" s="21" t="s">
-        <v>4704</v>
+        <v>4689</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="22"/>
-      <c r="B17" s="22"/>
-      <c r="C17" s="22"/>
+      <c r="A17" s="23"/>
+      <c r="B17" s="23"/>
+      <c r="C17" s="23"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="21" t="s">
-        <v>4705</v>
+        <v>4690</v>
       </c>
       <c r="B18" s="21" t="s">
-        <v>4706</v>
+        <v>4691</v>
       </c>
       <c r="C18" s="21" t="s">
-        <v>4707</v>
+        <v>4692</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="22"/>
-      <c r="B19" s="22"/>
-      <c r="C19" s="22"/>
+      <c r="A19" s="23"/>
+      <c r="B19" s="23"/>
+      <c r="C19" s="23"/>
     </row>
     <row r="20" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="15" t="s">
-        <v>4708</v>
+        <v>4693</v>
       </c>
       <c r="B20" s="13"/>
       <c r="C20" s="13" t="s">
-        <v>4709</v>
+        <v>4694</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="31.2" x14ac:dyDescent="0.25">
       <c r="A21" s="21" t="s">
-        <v>4710</v>
+        <v>4695</v>
       </c>
       <c r="B21" s="21" t="s">
-        <v>4711</v>
+        <v>4696</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>4712</v>
+        <v>4697</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="31.2" x14ac:dyDescent="0.25">
-      <c r="A22" s="25"/>
-      <c r="B22" s="25"/>
+      <c r="A22" s="22"/>
+      <c r="B22" s="22"/>
       <c r="C22" s="14" t="s">
-        <v>4713</v>
+        <v>4698</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="22"/>
-      <c r="B23" s="22"/>
+      <c r="A23" s="23"/>
+      <c r="B23" s="23"/>
       <c r="C23" s="13"/>
     </row>
     <row r="24" spans="1:3" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="21" t="s">
-        <v>4714</v>
+        <v>4699</v>
       </c>
       <c r="B24" s="21" t="s">
-        <v>4715</v>
+        <v>4700</v>
       </c>
       <c r="C24" s="21" t="s">
-        <v>4716</v>
+        <v>4701</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="22"/>
-      <c r="B25" s="22"/>
-      <c r="C25" s="22"/>
+      <c r="A25" s="23"/>
+      <c r="B25" s="23"/>
+      <c r="C25" s="23"/>
     </row>
     <row r="26" spans="1:3" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="21" t="s">
-        <v>4717</v>
+        <v>4702</v>
       </c>
       <c r="B26" s="21" t="s">
-        <v>4718</v>
+        <v>4703</v>
       </c>
       <c r="C26" s="21" t="s">
-        <v>4719</v>
+        <v>4704</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="22"/>
-      <c r="B27" s="22"/>
-      <c r="C27" s="22"/>
+      <c r="A27" s="23"/>
+      <c r="B27" s="23"/>
+      <c r="C27" s="23"/>
     </row>
     <row r="28" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="15" t="s">
-        <v>4720</v>
+        <v>4705</v>
       </c>
       <c r="B28" s="21"/>
       <c r="C28" s="21" t="s">
-        <v>4721</v>
+        <v>4706</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="15" t="s">
-        <v>4722</v>
-      </c>
-      <c r="B29" s="25"/>
-      <c r="C29" s="25"/>
+        <v>4707</v>
+      </c>
+      <c r="B29" s="22"/>
+      <c r="C29" s="22"/>
     </row>
     <row r="30" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="15" t="s">
-        <v>4723</v>
-      </c>
-      <c r="B30" s="25"/>
-      <c r="C30" s="25"/>
+        <v>4708</v>
+      </c>
+      <c r="B30" s="22"/>
+      <c r="C30" s="22"/>
     </row>
     <row r="31" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="15" t="s">
-        <v>4724</v>
-      </c>
-      <c r="B31" s="25"/>
-      <c r="C31" s="25"/>
+        <v>4709</v>
+      </c>
+      <c r="B31" s="22"/>
+      <c r="C31" s="22"/>
     </row>
     <row r="32" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="15" t="s">
-        <v>4725</v>
-      </c>
-      <c r="B32" s="25"/>
-      <c r="C32" s="25"/>
+        <v>4710</v>
+      </c>
+      <c r="B32" s="22"/>
+      <c r="C32" s="22"/>
     </row>
     <row r="33" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="15" t="s">
-        <v>4726</v>
-      </c>
-      <c r="B33" s="25"/>
-      <c r="C33" s="25"/>
+        <v>4711</v>
+      </c>
+      <c r="B33" s="22"/>
+      <c r="C33" s="22"/>
     </row>
     <row r="34" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="15" t="s">
-        <v>4727</v>
-      </c>
-      <c r="B34" s="22"/>
-      <c r="C34" s="22"/>
+        <v>4712</v>
+      </c>
+      <c r="B34" s="23"/>
+      <c r="C34" s="23"/>
     </row>
     <row r="35" spans="1:3" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A35" s="16" t="s">
-        <v>4728</v>
+        <v>4713</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="17" t="s">
-        <v>4730</v>
+        <v>4715</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="23" t="s">
-        <v>4682</v>
+      <c r="A39" s="24" t="s">
+        <v>4667</v>
       </c>
       <c r="B39" s="12" t="s">
-        <v>4683</v>
+        <v>4668</v>
       </c>
       <c r="C39" s="12"/>
     </row>
     <row r="40" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="24"/>
+      <c r="A40" s="25"/>
       <c r="B40" s="13" t="s">
-        <v>4684</v>
+        <v>4669</v>
       </c>
       <c r="C40" s="13" t="s">
-        <v>4685</v>
+        <v>4670</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="21" t="s">
-        <v>4731</v>
+        <v>4716</v>
       </c>
       <c r="B41" s="21" t="s">
-        <v>4732</v>
+        <v>4717</v>
       </c>
       <c r="C41" s="21" t="s">
-        <v>4733</v>
+        <v>4718</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="22"/>
-      <c r="B42" s="22"/>
-      <c r="C42" s="22"/>
+      <c r="A42" s="23"/>
+      <c r="B42" s="23"/>
+      <c r="C42" s="23"/>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="21" t="s">
-        <v>4734</v>
+        <v>4719</v>
       </c>
       <c r="B43" s="21" t="s">
-        <v>4735</v>
+        <v>4720</v>
       </c>
       <c r="C43" s="21" t="s">
-        <v>4736</v>
+        <v>4721</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="22"/>
-      <c r="B44" s="22"/>
-      <c r="C44" s="22"/>
+      <c r="A44" s="23"/>
+      <c r="B44" s="23"/>
+      <c r="C44" s="23"/>
     </row>
     <row r="45" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="15" t="s">
-        <v>4737</v>
+        <v>4722</v>
       </c>
       <c r="B45" s="21" t="s">
-        <v>4738</v>
+        <v>4723</v>
       </c>
       <c r="C45" s="21"/>
     </row>
     <row r="46" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="15" t="s">
-        <v>4739</v>
-      </c>
-      <c r="B46" s="25"/>
-      <c r="C46" s="25"/>
+        <v>4724</v>
+      </c>
+      <c r="B46" s="22"/>
+      <c r="C46" s="22"/>
     </row>
     <row r="47" spans="1:3" ht="31.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="15" t="s">
-        <v>4740</v>
-      </c>
-      <c r="B47" s="25"/>
-      <c r="C47" s="25"/>
+        <v>4725</v>
+      </c>
+      <c r="B47" s="22"/>
+      <c r="C47" s="22"/>
     </row>
     <row r="48" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="15" t="s">
-        <v>4741</v>
-      </c>
-      <c r="B48" s="25"/>
-      <c r="C48" s="25"/>
+        <v>4726</v>
+      </c>
+      <c r="B48" s="22"/>
+      <c r="C48" s="22"/>
     </row>
     <row r="49" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="15" t="s">
-        <v>4742</v>
-      </c>
-      <c r="B49" s="25"/>
-      <c r="C49" s="25"/>
+        <v>4727</v>
+      </c>
+      <c r="B49" s="22"/>
+      <c r="C49" s="22"/>
     </row>
     <row r="50" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="15" t="s">
-        <v>4743</v>
-      </c>
-      <c r="B50" s="25"/>
-      <c r="C50" s="25"/>
+        <v>4728</v>
+      </c>
+      <c r="B50" s="22"/>
+      <c r="C50" s="22"/>
     </row>
     <row r="51" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="15" t="s">
-        <v>4744</v>
-      </c>
-      <c r="B51" s="22"/>
-      <c r="C51" s="22"/>
+        <v>4729</v>
+      </c>
+      <c r="B51" s="23"/>
+      <c r="C51" s="23"/>
     </row>
     <row r="52" spans="1:3" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A52" s="16" t="s">
-        <v>4728</v>
+        <v>4713</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A54" s="18" t="s">
-        <v>4747</v>
+        <v>4732</v>
       </c>
     </row>
     <row r="55" spans="1:3" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A55" s="19" t="s">
-        <v>4748</v>
+        <v>4733</v>
       </c>
     </row>
     <row r="56" spans="1:3" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A56" s="19" t="s">
-        <v>4749</v>
+        <v>4734</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A57" s="19" t="s">
-        <v>4750</v>
+        <v>4735</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A58" s="19" t="s">
-        <v>4751</v>
+        <v>4736</v>
       </c>
     </row>
     <row r="59" spans="1:3" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A59" s="19" t="s">
-        <v>4752</v>
+        <v>4737</v>
       </c>
     </row>
     <row r="60" spans="1:3" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A60" s="19" t="s">
-        <v>4753</v>
+        <v>4738</v>
       </c>
     </row>
     <row r="61" spans="1:3" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A61" s="19" t="s">
-        <v>4754</v>
+        <v>4739</v>
       </c>
     </row>
     <row r="62" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
@@ -15784,14 +15859,26 @@
     </row>
   </sheetData>
   <mergeCells count="42">
-    <mergeCell ref="B45:B51"/>
-    <mergeCell ref="C45:C51"/>
-    <mergeCell ref="A41:A42"/>
-    <mergeCell ref="B41:B42"/>
-    <mergeCell ref="C41:C42"/>
-    <mergeCell ref="A43:A44"/>
-    <mergeCell ref="B43:B44"/>
-    <mergeCell ref="C43:C44"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C9"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="B6:B7"/>
     <mergeCell ref="A39:A40"/>
     <mergeCell ref="A18:A19"/>
     <mergeCell ref="B18:B19"/>
@@ -15806,26 +15893,14 @@
     <mergeCell ref="C26:C27"/>
     <mergeCell ref="B28:B34"/>
     <mergeCell ref="C28:C34"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C9"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="B45:B51"/>
+    <mergeCell ref="C45:C51"/>
+    <mergeCell ref="A41:A42"/>
+    <mergeCell ref="B41:B42"/>
+    <mergeCell ref="C41:C42"/>
+    <mergeCell ref="A43:A44"/>
+    <mergeCell ref="B43:B44"/>
+    <mergeCell ref="C43:C44"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -15836,7 +15911,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0111484F-11D4-4F10-BD6F-922F3BE2F87B}">
   <dimension ref="A1:K60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
@@ -77226,8 +77301,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9597344-7039-47C2-9649-74AC60EC1426}">
   <dimension ref="A1:S150"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P22" sqref="P22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -77241,7 +77316,7 @@
     <col min="11" max="12" width="22.33203125" style="3" customWidth="1"/>
     <col min="13" max="13" width="8.88671875" style="3"/>
     <col min="14" max="14" width="3.109375" style="3" customWidth="1"/>
-    <col min="15" max="15" width="21.77734375" style="3" customWidth="1"/>
+    <col min="15" max="15" width="52.5546875" style="3" customWidth="1"/>
     <col min="16" max="16" width="13.21875" style="3" customWidth="1"/>
     <col min="17" max="17" width="12.6640625" style="3" customWidth="1"/>
     <col min="18" max="16384" width="8.88671875" style="3"/>
@@ -77252,12 +77327,12 @@
         <v>4509</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>4757</v>
+        <v>4742</v>
       </c>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
       <c r="J1" s="2" t="s">
-        <v>4679</v>
+        <v>4664</v>
       </c>
       <c r="N1" s="2" t="s">
         <v>4508</v>
@@ -77275,16 +77350,16 @@
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2" t="s">
-        <v>4758</v>
+        <v>4743</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>4759</v>
+        <v>4744</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>4806</v>
+        <v>4791</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>4807</v>
+        <v>4792</v>
       </c>
       <c r="I2" s="2"/>
       <c r="J2" s="2" t="s">
@@ -77318,16 +77393,16 @@
         <v>2578</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>4599</v>
+        <v>4584</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>4678</v>
+        <v>4663</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>4760</v>
+        <v>4745</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>4761</v>
+        <v>4746</v>
       </c>
       <c r="G3" s="3">
         <v>10</v>
@@ -77339,10 +77414,10 @@
         <v>4516</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>4523</v>
+        <v>4800</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>4536</v>
+        <v>4521</v>
       </c>
       <c r="N3">
         <v>0</v>
@@ -77351,10 +77426,10 @@
         <v>4491</v>
       </c>
       <c r="P3" s="9">
-        <v>0.56786998596961302</v>
+        <v>0.56701773752585505</v>
       </c>
       <c r="Q3" s="9">
-        <v>5.1675372339485902E-2</v>
+        <v>6.03786344143694E-2</v>
       </c>
       <c r="R3">
         <v>10</v>
@@ -77368,16 +77443,16 @@
         <v>2319</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>4600</v>
+        <v>4585</v>
       </c>
       <c r="C4" s="10" t="s">
         <v>3467</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>4762</v>
+        <v>4747</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>4761</v>
+        <v>4746</v>
       </c>
       <c r="G4" s="3">
         <v>-10</v>
@@ -77389,10 +77464,10 @@
         <v>4517</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>4524</v>
+        <v>4801</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>4537</v>
+        <v>4522</v>
       </c>
       <c r="N4">
         <v>1</v>
@@ -77401,10 +77476,10 @@
         <v>4493</v>
       </c>
       <c r="P4" s="9">
-        <v>0.56947563841830195</v>
+        <v>0.56986074837748002</v>
       </c>
       <c r="Q4" s="9">
-        <v>3.5275935631025601E-2</v>
+        <v>3.1341949551330898E-2</v>
       </c>
       <c r="R4">
         <v>10</v>
@@ -77415,7 +77490,7 @@
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>4548</v>
+        <v>4533</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>2341</v>
@@ -77427,7 +77502,7 @@
         <v>3730</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>4763</v>
+        <v>4748</v>
       </c>
       <c r="G5" s="3">
         <v>0.18468000000000001</v>
@@ -77439,10 +77514,10 @@
         <v>4518</v>
       </c>
       <c r="K5" s="3" t="s">
-        <v>4525</v>
+        <v>4802</v>
       </c>
       <c r="L5" s="3" t="s">
-        <v>4538</v>
+        <v>4523</v>
       </c>
       <c r="N5">
         <v>2</v>
@@ -77451,10 +77526,10 @@
         <v>4494</v>
       </c>
       <c r="P5" s="9">
-        <v>0.56983653938633305</v>
+        <v>0.56938095593448801</v>
       </c>
       <c r="Q5" s="9">
-        <v>3.15898498980349E-2</v>
+        <v>3.6242241071090697E-2</v>
       </c>
       <c r="R5">
         <v>10</v>
@@ -77468,13 +77543,13 @@
         <v>3730</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>4601</v>
+        <v>4586</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>4673</v>
+        <v>4658</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>4763</v>
+        <v>4748</v>
       </c>
       <c r="G6" s="3">
         <v>-0.25131000000000003</v>
@@ -77486,10 +77561,10 @@
         <v>4519</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>4526</v>
+        <v>4794</v>
       </c>
       <c r="L6" s="3" t="s">
-        <v>4539</v>
+        <v>4524</v>
       </c>
       <c r="N6">
         <v>3</v>
@@ -77498,10 +77573,10 @@
         <v>4495</v>
       </c>
       <c r="P6" s="9">
-        <v>0.57149999806731899</v>
+        <v>0.57150000437152304</v>
       </c>
       <c r="Q6" s="9">
-        <v>1.4600005440574101E-2</v>
+        <v>1.45996428233513E-2</v>
       </c>
       <c r="R6">
         <v>10</v>
@@ -77512,16 +77587,16 @@
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>4549</v>
+        <v>4534</v>
       </c>
       <c r="B7" s="10" t="s">
         <v>2384</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>4764</v>
+        <v>4749</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>4763</v>
+        <v>4748</v>
       </c>
       <c r="G7" s="3">
         <v>0.18468000000000001</v>
@@ -77533,10 +77608,10 @@
         <v>4520</v>
       </c>
       <c r="K7" s="3" t="s">
-        <v>4527</v>
+        <v>4795</v>
       </c>
       <c r="L7" s="3" t="s">
-        <v>4540</v>
+        <v>4525</v>
       </c>
       <c r="N7">
         <v>4</v>
@@ -77545,7 +77620,7 @@
         <v>4496</v>
       </c>
       <c r="P7" s="9">
-        <v>0.5714999986</v>
+        <v>0.57149996940000003</v>
       </c>
       <c r="Q7" s="9">
         <v>1.46E-2</v>
@@ -77559,7 +77634,7 @@
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>4550</v>
+        <v>4535</v>
       </c>
       <c r="B8" s="10" t="s">
         <v>2485</v>
@@ -77568,7 +77643,7 @@
         <v>2977</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>4765</v>
+        <v>4750</v>
       </c>
       <c r="G8" s="3">
         <v>4.5421999999999993</v>
@@ -77576,14 +77651,11 @@
       <c r="H8" s="3">
         <v>5.0640999999999998</v>
       </c>
-      <c r="J8" s="3" t="s">
-        <v>4521</v>
-      </c>
       <c r="K8" s="3" t="s">
-        <v>4528</v>
+        <v>4799</v>
       </c>
       <c r="L8" s="3" t="s">
-        <v>4541</v>
+        <v>4526</v>
       </c>
       <c r="N8">
         <v>5</v>
@@ -77592,10 +77664,10 @@
         <v>4497</v>
       </c>
       <c r="P8" s="9">
-        <v>0.57149999856254097</v>
+        <v>0.56756653924207201</v>
       </c>
       <c r="Q8" s="9">
-        <v>1.46000003825917E-2</v>
+        <v>5.47735265488902E-2</v>
       </c>
       <c r="R8">
         <v>10</v>
@@ -77612,10 +77684,10 @@
         <v>2526</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>4766</v>
+        <v>4751</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>4767</v>
+        <v>4752</v>
       </c>
       <c r="G9" s="3">
         <v>7.4516000000000009</v>
@@ -77623,14 +77695,11 @@
       <c r="H9" s="3">
         <v>7.7523999999999997</v>
       </c>
-      <c r="J9" s="3" t="s">
-        <v>4522</v>
-      </c>
       <c r="K9" s="3" t="s">
-        <v>4529</v>
+        <v>4797</v>
       </c>
       <c r="L9" s="3" t="s">
-        <v>4542</v>
+        <v>4527</v>
       </c>
       <c r="N9">
         <v>6</v>
@@ -77639,10 +77708,10 @@
         <v>4498</v>
       </c>
       <c r="P9" s="9">
-        <v>0.56937751147897298</v>
+        <v>0.568558824474936</v>
       </c>
       <c r="Q9" s="9">
-        <v>3.6278161568669302E-2</v>
+        <v>4.4638963191713503E-2</v>
       </c>
       <c r="R9">
         <v>10</v>
@@ -77653,16 +77722,16 @@
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>4551</v>
+        <v>4536</v>
       </c>
       <c r="B10" s="10" t="s">
         <v>2300</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>4768</v>
+        <v>4753</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>4769</v>
+        <v>4754</v>
       </c>
       <c r="G10" s="3">
         <v>7.4516000000000009</v>
@@ -77671,10 +77740,10 @@
         <v>7.7523999999999997</v>
       </c>
       <c r="K10" s="3" t="s">
-        <v>4530</v>
+        <v>4798</v>
       </c>
       <c r="L10" s="3" t="s">
-        <v>4543</v>
+        <v>4528</v>
       </c>
       <c r="N10">
         <v>7</v>
@@ -77683,10 +77752,10 @@
         <v>4499</v>
       </c>
       <c r="P10" s="9">
-        <v>0.56597185735775601</v>
+        <v>0.564623362864902</v>
       </c>
       <c r="Q10" s="9">
-        <v>5.3128116916555897E-2</v>
+        <v>6.2525220591307704E-2</v>
       </c>
       <c r="R10">
         <v>10</v>
@@ -77706,7 +77775,7 @@
         <v>3499</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>4770</v>
+        <v>4755</v>
       </c>
       <c r="G11" s="3">
         <v>7.2302000000000008</v>
@@ -77715,10 +77784,10 @@
         <v>7.5379000000000005</v>
       </c>
       <c r="K11" s="3" t="s">
-        <v>4531</v>
+        <v>4803</v>
       </c>
       <c r="L11" s="3" t="s">
-        <v>4544</v>
+        <v>4529</v>
       </c>
       <c r="N11">
         <v>8</v>
@@ -77727,10 +77796,10 @@
         <v>4501</v>
       </c>
       <c r="P11" s="9">
-        <v>0.56587473475158301</v>
+        <v>0.56449988772161697</v>
       </c>
       <c r="Q11" s="9">
-        <v>5.32024503092072E-2</v>
+        <v>6.2635917567891303E-2</v>
       </c>
       <c r="R11">
         <v>10</v>
@@ -77741,7 +77810,7 @@
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>4552</v>
+        <v>4537</v>
       </c>
       <c r="B12" s="10" t="s">
         <v>3325</v>
@@ -77750,7 +77819,7 @@
         <v>3022</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>4771</v>
+        <v>4756</v>
       </c>
       <c r="G12" s="3">
         <v>0.18468000000000001</v>
@@ -77759,10 +77828,10 @@
         <v>0.25131000000000003</v>
       </c>
       <c r="K12" s="3" t="s">
-        <v>4532</v>
+        <v>4804</v>
       </c>
       <c r="L12" s="3" t="s">
-        <v>4545</v>
+        <v>4530</v>
       </c>
       <c r="N12">
         <v>9</v>
@@ -77771,10 +77840,10 @@
         <v>4502</v>
       </c>
       <c r="P12" s="9">
-        <v>0.566702277452658</v>
+        <v>0.56554896440046498</v>
       </c>
       <c r="Q12" s="9">
-        <v>5.2569085339229403E-2</v>
+        <v>6.1695407490629302E-2</v>
       </c>
       <c r="R12">
         <v>10</v>
@@ -77788,13 +77857,13 @@
         <v>4053</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>4602</v>
+        <v>4587</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>3015</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>4772</v>
+        <v>4757</v>
       </c>
       <c r="G13" s="3">
         <v>16.378999999999998</v>
@@ -77803,10 +77872,10 @@
         <v>16.997999999999998</v>
       </c>
       <c r="K13" s="3" t="s">
-        <v>4533</v>
+        <v>4805</v>
       </c>
       <c r="L13" s="3" t="s">
-        <v>4546</v>
+        <v>4531</v>
       </c>
       <c r="N13">
         <v>10</v>
@@ -77815,10 +77884,10 @@
         <v>4503</v>
       </c>
       <c r="P13" s="9">
-        <v>0.56883192376911695</v>
+        <v>0.56932705181502696</v>
       </c>
       <c r="Q13" s="9">
-        <v>3.5715102856129201E-2</v>
+        <v>3.1796165175177103E-2</v>
       </c>
       <c r="R13">
         <v>10</v>
@@ -77829,16 +77898,16 @@
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
-        <v>4756</v>
+        <v>4741</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>4603</v>
+        <v>4588</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>3344</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>4772</v>
+        <v>4757</v>
       </c>
       <c r="G14" s="3">
         <v>16.378999999999998</v>
@@ -77847,10 +77916,10 @@
         <v>16.997999999999998</v>
       </c>
       <c r="K14" s="3" t="s">
-        <v>4534</v>
+        <v>4796</v>
       </c>
       <c r="L14" s="3" t="s">
-        <v>4547</v>
+        <v>4532</v>
       </c>
       <c r="N14">
         <v>11</v>
@@ -77859,10 +77928,10 @@
         <v>4504</v>
       </c>
       <c r="P14" s="9">
-        <v>0.56870259396300804</v>
+        <v>0.56760453530985799</v>
       </c>
       <c r="Q14" s="9">
-        <v>3.6738616605739197E-2</v>
+        <v>4.54279139224147E-2</v>
       </c>
       <c r="R14">
         <v>10</v>
@@ -77873,7 +77942,7 @@
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A15" s="10" t="s">
-        <v>4553</v>
+        <v>4538</v>
       </c>
       <c r="B15" s="10" t="s">
         <v>2636</v>
@@ -77882,7 +77951,7 @@
         <v>2882</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>4773</v>
+        <v>4758</v>
       </c>
       <c r="G15" s="3">
         <v>16.378999999999998</v>
@@ -77891,7 +77960,7 @@
         <v>16.997999999999998</v>
       </c>
       <c r="K15" s="3" t="s">
-        <v>4535</v>
+        <v>4808</v>
       </c>
       <c r="N15">
         <v>12</v>
@@ -77900,10 +77969,10 @@
         <v>4505</v>
       </c>
       <c r="P15" s="9">
-        <v>0.56895874618230402</v>
+        <v>0.568242394820476</v>
       </c>
       <c r="Q15" s="9">
-        <v>3.2311142880910401E-2</v>
+        <v>3.7303025007249802E-2</v>
       </c>
       <c r="R15">
         <v>10</v>
@@ -77914,16 +77983,16 @@
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A16" s="10" t="s">
-        <v>4554</v>
+        <v>4539</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>4604</v>
+        <v>4589</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>2906</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>4773</v>
+        <v>4758</v>
       </c>
       <c r="G16" s="3">
         <v>16.378999999999998</v>
@@ -77931,6 +78000,9 @@
       <c r="H16" s="3">
         <v>16.997999999999998</v>
       </c>
+      <c r="K16" s="3" t="s">
+        <v>4811</v>
+      </c>
       <c r="N16">
         <v>13</v>
       </c>
@@ -77938,10 +78010,10 @@
         <v>4506</v>
       </c>
       <c r="P16" s="9">
-        <v>0.569297183610879</v>
+        <v>0.56868308314960703</v>
       </c>
       <c r="Q16" s="9">
-        <v>3.2033044871883097E-2</v>
+        <v>3.6892440898376601E-2</v>
       </c>
       <c r="R16">
         <v>10</v>
@@ -77952,7 +78024,7 @@
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A17" s="10" t="s">
-        <v>4555</v>
+        <v>4540</v>
       </c>
       <c r="B17" s="11" t="s">
         <v>2701</v>
@@ -77961,7 +78033,7 @@
         <v>3411</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>4774</v>
+        <v>4759</v>
       </c>
       <c r="G17" s="3">
         <v>16.378999999999998</v>
@@ -77969,6 +78041,9 @@
       <c r="H17" s="3">
         <v>16.997999999999998</v>
       </c>
+      <c r="K17" s="3" t="s">
+        <v>4807</v>
+      </c>
       <c r="N17">
         <v>14</v>
       </c>
@@ -77976,10 +78051,10 @@
         <v>4507</v>
       </c>
       <c r="P17" s="9">
-        <v>0.56828233874295198</v>
+        <v>0.56700552941257198</v>
       </c>
       <c r="Q17" s="9">
-        <v>3.7025331098022501E-2</v>
+        <v>4.5923137129019603E-2</v>
       </c>
       <c r="R17">
         <v>10</v>
@@ -77990,7 +78065,7 @@
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A18" s="10" t="s">
-        <v>4556</v>
+        <v>4541</v>
       </c>
       <c r="B18" s="11" t="s">
         <v>2704</v>
@@ -78001,7 +78076,7 @@
         <v>2974</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>4775</v>
+        <v>4760</v>
       </c>
       <c r="G18" s="4">
         <v>4.9359000000000002</v>
@@ -78010,11 +78085,13 @@
         <v>5.4578000000000007</v>
       </c>
       <c r="I18" s="4"/>
-      <c r="K18" s="4"/>
+      <c r="K18" s="3" t="s">
+        <v>4810</v>
+      </c>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A19" s="10" t="s">
-        <v>4557</v>
+        <v>4542</v>
       </c>
       <c r="B19" s="11" t="s">
         <v>2707</v>
@@ -78025,7 +78102,7 @@
         <v>3933</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>4775</v>
+        <v>4760</v>
       </c>
       <c r="G19" s="4">
         <v>4.9359000000000002</v>
@@ -78034,11 +78111,13 @@
         <v>5.4578000000000007</v>
       </c>
       <c r="I19" s="4"/>
-      <c r="K19" s="4"/>
+      <c r="K19" s="3" t="s">
+        <v>4806</v>
+      </c>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A20" s="10" t="s">
-        <v>4558</v>
+        <v>4543</v>
       </c>
       <c r="B20" s="11" t="s">
         <v>2724</v>
@@ -78049,7 +78128,7 @@
         <v>3340</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>4776</v>
+        <v>4761</v>
       </c>
       <c r="G20" s="4">
         <v>4.9359000000000002</v>
@@ -78058,11 +78137,13 @@
         <v>5.4578000000000007</v>
       </c>
       <c r="I20" s="4"/>
-      <c r="K20" s="4"/>
+      <c r="K20" s="3" t="s">
+        <v>4809</v>
+      </c>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A21" s="10" t="s">
-        <v>4559</v>
+        <v>4544</v>
       </c>
       <c r="B21" s="11" t="s">
         <v>2323</v>
@@ -78073,7 +78154,7 @@
         <v>3428</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>4777</v>
+        <v>4762</v>
       </c>
       <c r="G21" s="4">
         <v>1.6609000000000003</v>
@@ -78082,14 +78163,16 @@
         <v>1.8349</v>
       </c>
       <c r="I21" s="4"/>
-      <c r="K21" s="4"/>
+      <c r="K21" s="3" t="s">
+        <v>4817</v>
+      </c>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A22" s="10" t="s">
-        <v>4560</v>
+        <v>4545</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>4605</v>
+        <v>4590</v>
       </c>
       <c r="C22" s="4"/>
       <c r="D22" s="4"/>
@@ -78097,7 +78180,7 @@
         <v>2348</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>4778</v>
+        <v>4763</v>
       </c>
       <c r="G22" s="4">
         <v>3.2749999999999999</v>
@@ -78106,11 +78189,13 @@
         <v>3.6229999999999998</v>
       </c>
       <c r="I22" s="4"/>
-      <c r="K22" s="4"/>
+      <c r="K22" s="3" t="s">
+        <v>4818</v>
+      </c>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A23" s="10" t="s">
-        <v>4561</v>
+        <v>4546</v>
       </c>
       <c r="B23" s="11" t="s">
         <v>2755</v>
@@ -78118,10 +78203,10 @@
       <c r="C23" s="4"/>
       <c r="D23" s="4"/>
       <c r="E23" s="3" t="s">
-        <v>4779</v>
+        <v>4764</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>4780</v>
+        <v>4765</v>
       </c>
       <c r="G23" s="4">
         <v>1.6609000000000003</v>
@@ -78130,22 +78215,24 @@
         <v>1.8349</v>
       </c>
       <c r="I23" s="4"/>
-      <c r="K23" s="4"/>
+      <c r="K23" s="3" t="s">
+        <v>4819</v>
+      </c>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A24" s="10" t="s">
-        <v>4562</v>
+        <v>4547</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>4606</v>
+        <v>4591</v>
       </c>
       <c r="C24" s="4"/>
       <c r="D24" s="4"/>
       <c r="E24" s="3" t="s">
-        <v>4781</v>
+        <v>4766</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>4782</v>
+        <v>4767</v>
       </c>
       <c r="G24" s="4">
         <v>1.6140000000000001</v>
@@ -78154,22 +78241,24 @@
         <v>1.7882000000000002</v>
       </c>
       <c r="I24" s="4"/>
-      <c r="K24" s="4"/>
+      <c r="K24" s="3" t="s">
+        <v>4812</v>
+      </c>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A25" s="10" t="s">
-        <v>4563</v>
+        <v>4548</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>4607</v>
+        <v>4592</v>
       </c>
       <c r="C25" s="4"/>
       <c r="D25" s="4"/>
       <c r="E25" s="3" t="s">
-        <v>4783</v>
+        <v>4768</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>4784</v>
+        <v>4769</v>
       </c>
       <c r="G25" s="4">
         <v>1.6011887820195003</v>
@@ -78178,74 +78267,82 @@
         <v>1.8349</v>
       </c>
       <c r="I25" s="4"/>
-      <c r="K25" s="4"/>
+      <c r="K25" s="3" t="s">
+        <v>4813</v>
+      </c>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A26" s="10" t="s">
-        <v>4564</v>
+        <v>4549</v>
       </c>
       <c r="B26" s="11" t="s">
-        <v>4608</v>
+        <v>4593</v>
       </c>
       <c r="C26" s="4"/>
       <c r="D26" s="4"/>
       <c r="E26" s="3" t="s">
-        <v>4785</v>
+        <v>4770</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>4786</v>
+        <v>4771</v>
       </c>
       <c r="G26" s="4"/>
       <c r="H26" s="4"/>
       <c r="I26" s="4"/>
-      <c r="K26" s="4"/>
+      <c r="K26" s="3" t="s">
+        <v>4816</v>
+      </c>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A27" s="10" t="s">
-        <v>4565</v>
+        <v>4550</v>
       </c>
       <c r="B27" s="11" t="s">
-        <v>4609</v>
+        <v>4594</v>
       </c>
       <c r="C27" s="4"/>
       <c r="D27" s="4"/>
       <c r="E27" s="3" t="s">
-        <v>4787</v>
+        <v>4772</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>4786</v>
+        <v>4771</v>
       </c>
       <c r="G27" s="4"/>
       <c r="H27" s="4"/>
       <c r="I27" s="4"/>
-      <c r="K27" s="4"/>
+      <c r="K27" s="3" t="s">
+        <v>4814</v>
+      </c>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A28" s="10" t="s">
-        <v>4566</v>
+        <v>4551</v>
       </c>
       <c r="B28" s="11" t="s">
-        <v>4610</v>
+        <v>4595</v>
       </c>
       <c r="C28" s="4"/>
       <c r="D28" s="4"/>
       <c r="E28" s="3" t="s">
-        <v>4552</v>
+        <v>4537</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>4786</v>
+        <v>4771</v>
       </c>
       <c r="G28" s="4"/>
       <c r="H28" s="4"/>
       <c r="I28" s="4"/>
-      <c r="K28" s="4"/>
+      <c r="K28" s="3" t="s">
+        <v>4815</v>
+      </c>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A29" s="10" t="s">
-        <v>4567</v>
+        <v>4552</v>
       </c>
       <c r="B29" s="11" t="s">
-        <v>4611</v>
+        <v>4596</v>
       </c>
       <c r="C29" s="4"/>
       <c r="D29" s="4"/>
@@ -78253,7 +78350,7 @@
         <v>3397</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>4788</v>
+        <v>4773</v>
       </c>
       <c r="G29" s="4">
         <v>3.7923</v>
@@ -78262,14 +78359,16 @@
         <v>5.2276000000000007</v>
       </c>
       <c r="I29" s="4"/>
-      <c r="K29" s="4"/>
+      <c r="K29" s="3" t="s">
+        <v>4822</v>
+      </c>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A30" s="10" t="s">
-        <v>4568</v>
+        <v>4553</v>
       </c>
       <c r="B30" s="11" t="s">
-        <v>4612</v>
+        <v>4597</v>
       </c>
       <c r="C30" s="4"/>
       <c r="D30" s="4"/>
@@ -78277,7 +78376,7 @@
         <v>3402</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>4789</v>
+        <v>4774</v>
       </c>
       <c r="G30" s="4">
         <v>16.116</v>
@@ -78286,14 +78385,16 @@
         <v>16.783999999999999</v>
       </c>
       <c r="I30" s="4"/>
-      <c r="K30" s="4"/>
+      <c r="K30" s="3" t="s">
+        <v>4821</v>
+      </c>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A31" s="10" t="s">
-        <v>4569</v>
+        <v>4554</v>
       </c>
       <c r="B31" s="11" t="s">
-        <v>4613</v>
+        <v>4598</v>
       </c>
       <c r="C31" s="4"/>
       <c r="D31" s="4"/>
@@ -78301,7 +78402,7 @@
         <v>2812</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>4790</v>
+        <v>4775</v>
       </c>
       <c r="G31" s="4">
         <v>16.116</v>
@@ -78310,11 +78411,13 @@
         <v>16.783999999999999</v>
       </c>
       <c r="I31" s="4"/>
-      <c r="K31" s="4"/>
+      <c r="K31" s="3" t="s">
+        <v>4825</v>
+      </c>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A32" s="10" t="s">
-        <v>4570</v>
+        <v>4555</v>
       </c>
       <c r="B32" s="11" t="s">
         <v>2767</v>
@@ -78322,10 +78425,10 @@
       <c r="C32" s="4"/>
       <c r="D32" s="4"/>
       <c r="E32" s="3" t="s">
-        <v>4599</v>
+        <v>4584</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>4791</v>
+        <v>4776</v>
       </c>
       <c r="G32" s="4">
         <v>9.4116</v>
@@ -78334,22 +78437,24 @@
         <v>11.068000000000001</v>
       </c>
       <c r="I32" s="4"/>
-      <c r="K32" s="4"/>
+      <c r="K32" s="3" t="s">
+        <v>4824</v>
+      </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33" s="10" t="s">
-        <v>4571</v>
+        <v>4556</v>
       </c>
       <c r="B33" s="11" t="s">
-        <v>4614</v>
+        <v>4599</v>
       </c>
       <c r="C33" s="4"/>
       <c r="D33" s="4"/>
       <c r="E33" s="3" t="s">
-        <v>4602</v>
+        <v>4587</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>4791</v>
+        <v>4776</v>
       </c>
       <c r="G33" s="4">
         <v>9.4116</v>
@@ -78358,14 +78463,16 @@
         <v>11.068000000000001</v>
       </c>
       <c r="I33" s="4"/>
-      <c r="K33" s="4"/>
+      <c r="K33" s="3" t="s">
+        <v>4820</v>
+      </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A34" s="10" t="s">
-        <v>4572</v>
+        <v>4557</v>
       </c>
       <c r="B34" s="11" t="s">
-        <v>4615</v>
+        <v>4600</v>
       </c>
       <c r="C34" s="4"/>
       <c r="D34" s="4"/>
@@ -78373,19 +78480,21 @@
         <v>3158</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>4792</v>
+        <v>4777</v>
       </c>
       <c r="G34" s="4"/>
       <c r="H34" s="4"/>
       <c r="I34" s="4"/>
-      <c r="K34" s="4"/>
+      <c r="K34" s="3" t="s">
+        <v>4823</v>
+      </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A35" s="10" t="s">
-        <v>4573</v>
+        <v>4558</v>
       </c>
       <c r="B35" s="11" t="s">
-        <v>4616</v>
+        <v>4601</v>
       </c>
       <c r="C35" s="4"/>
       <c r="D35" s="4"/>
@@ -78393,27 +78502,29 @@
         <v>3687</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>4792</v>
+        <v>4777</v>
       </c>
       <c r="G35" s="4"/>
       <c r="H35" s="4"/>
       <c r="I35" s="4"/>
-      <c r="K35" s="4"/>
+      <c r="K35" s="3" t="s">
+        <v>4832</v>
+      </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A36" s="10" t="s">
-        <v>4574</v>
+        <v>4559</v>
       </c>
       <c r="B36" s="11" t="s">
-        <v>4617</v>
+        <v>4602</v>
       </c>
       <c r="C36" s="4"/>
       <c r="D36" s="4"/>
       <c r="E36" s="3" t="s">
-        <v>4600</v>
+        <v>4585</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>4793</v>
+        <v>4778</v>
       </c>
       <c r="G36" s="4">
         <v>9.4116</v>
@@ -78422,11 +78533,13 @@
         <v>11.068000000000001</v>
       </c>
       <c r="I36" s="4"/>
-      <c r="K36" s="4"/>
+      <c r="K36" s="3" t="s">
+        <v>4833</v>
+      </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A37" s="10" t="s">
-        <v>4575</v>
+        <v>4560</v>
       </c>
       <c r="B37" s="11" t="s">
         <v>2297</v>
@@ -78434,10 +78547,10 @@
       <c r="C37" s="4"/>
       <c r="D37" s="4"/>
       <c r="E37" s="3" t="s">
-        <v>4603</v>
+        <v>4588</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>4793</v>
+        <v>4778</v>
       </c>
       <c r="G37" s="4">
         <v>9.4116</v>
@@ -78446,14 +78559,16 @@
         <v>11.068000000000001</v>
       </c>
       <c r="I37" s="4"/>
-      <c r="K37" s="4"/>
+      <c r="K37" s="3" t="s">
+        <v>4826</v>
+      </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A38" s="10" t="s">
-        <v>4576</v>
+        <v>4561</v>
       </c>
       <c r="B38" s="11" t="s">
-        <v>4618</v>
+        <v>4603</v>
       </c>
       <c r="C38" s="4"/>
       <c r="D38" s="4"/>
@@ -78461,7 +78576,7 @@
         <v>3173</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>4793</v>
+        <v>4778</v>
       </c>
       <c r="G38" s="4">
         <v>9.4116</v>
@@ -78470,11 +78585,13 @@
         <v>11.068000000000001</v>
       </c>
       <c r="I38" s="4"/>
-      <c r="K38" s="4"/>
+      <c r="K38" s="3" t="s">
+        <v>4827</v>
+      </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A39" s="10" t="s">
-        <v>4577</v>
+        <v>4562</v>
       </c>
       <c r="B39" s="11" t="s">
         <v>2834</v>
@@ -78485,7 +78602,7 @@
         <v>3467</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>4794</v>
+        <v>4779</v>
       </c>
       <c r="G39" s="4">
         <v>9.4116</v>
@@ -78494,22 +78611,24 @@
         <v>11.068000000000001</v>
       </c>
       <c r="I39" s="4"/>
-      <c r="K39" s="4"/>
+      <c r="K39" s="3" t="s">
+        <v>4828</v>
+      </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A40" s="10" t="s">
-        <v>4578</v>
+        <v>4563</v>
       </c>
       <c r="B40" s="11" t="s">
-        <v>4619</v>
+        <v>4604</v>
       </c>
       <c r="C40" s="4"/>
       <c r="D40" s="4"/>
       <c r="E40" s="3" t="s">
-        <v>4678</v>
+        <v>4663</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>4795</v>
+        <v>4780</v>
       </c>
       <c r="G40" s="4">
         <v>9.4116</v>
@@ -78518,14 +78637,16 @@
         <v>11.068000000000001</v>
       </c>
       <c r="I40" s="4"/>
-      <c r="K40" s="4"/>
+      <c r="K40" s="3" t="s">
+        <v>4829</v>
+      </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A41" s="10" t="s">
-        <v>4579</v>
+        <v>4564</v>
       </c>
       <c r="B41" s="11" t="s">
-        <v>4620</v>
+        <v>4605</v>
       </c>
       <c r="C41" s="4"/>
       <c r="D41" s="4"/>
@@ -78533,7 +78654,7 @@
         <v>3212</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>4796</v>
+        <v>4781</v>
       </c>
       <c r="G41" s="4">
         <v>16.116</v>
@@ -78542,11 +78663,13 @@
         <v>16.783999999999999</v>
       </c>
       <c r="I41" s="4"/>
-      <c r="K41" s="4"/>
+      <c r="K41" s="3" t="s">
+        <v>4830</v>
+      </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A42" s="10" t="s">
-        <v>4580</v>
+        <v>4565</v>
       </c>
       <c r="B42" s="11" t="s">
         <v>4009</v>
@@ -78557,7 +78680,7 @@
         <v>4053</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>4797</v>
+        <v>4782</v>
       </c>
       <c r="G42" s="4">
         <v>5.1994999999999996</v>
@@ -78566,14 +78689,16 @@
         <v>6.7501000000000007</v>
       </c>
       <c r="I42" s="4"/>
-      <c r="K42" s="4"/>
+      <c r="K42" s="3" t="s">
+        <v>4831</v>
+      </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A43" s="10" t="s">
-        <v>4581</v>
+        <v>4566</v>
       </c>
       <c r="B43" s="11" t="s">
-        <v>4621</v>
+        <v>4606</v>
       </c>
       <c r="C43" s="4"/>
       <c r="D43" s="4"/>
@@ -78581,7 +78706,7 @@
         <v>4325</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>4798</v>
+        <v>4783</v>
       </c>
       <c r="G43" s="4">
         <v>-11.154</v>
@@ -78590,11 +78715,10 @@
         <v>-9.6391000000000009</v>
       </c>
       <c r="I43" s="4"/>
-      <c r="K43" s="4"/>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A44" s="10" t="s">
-        <v>4582</v>
+        <v>4567</v>
       </c>
       <c r="B44" s="11" t="s">
         <v>3238</v>
@@ -78605,7 +78729,7 @@
         <v>3680</v>
       </c>
       <c r="F44" s="3" t="s">
-        <v>4799</v>
+        <v>4784</v>
       </c>
       <c r="G44" s="4">
         <v>11.484999999999999</v>
@@ -78614,22 +78738,21 @@
         <v>12.918000000000001</v>
       </c>
       <c r="I44" s="4"/>
-      <c r="K44" s="4"/>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A45" s="10" t="s">
-        <v>4583</v>
+        <v>4568</v>
       </c>
       <c r="B45" s="10" t="s">
-        <v>4622</v>
+        <v>4607</v>
       </c>
       <c r="C45" s="4"/>
       <c r="D45" s="4"/>
       <c r="E45" s="3" t="s">
-        <v>4800</v>
+        <v>4785</v>
       </c>
       <c r="F45" s="3" t="s">
-        <v>4801</v>
+        <v>4786</v>
       </c>
       <c r="G45" s="4">
         <v>5.4433999999999996</v>
@@ -78638,20 +78761,19 @@
         <v>6.9834000000000005</v>
       </c>
       <c r="I45" s="4"/>
-      <c r="K45" s="4"/>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A46" s="10" t="s">
-        <v>4584</v>
+        <v>4569</v>
       </c>
       <c r="B46" s="10" t="s">
-        <v>4623</v>
+        <v>4608</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>4802</v>
+        <v>4787</v>
       </c>
       <c r="F46" s="3" t="s">
-        <v>4803</v>
+        <v>4788</v>
       </c>
       <c r="G46" s="3">
         <v>30.903600000000001</v>
@@ -78662,16 +78784,16 @@
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A47" s="10" t="s">
-        <v>4585</v>
+        <v>4570</v>
       </c>
       <c r="B47" s="10" t="s">
-        <v>4624</v>
+        <v>4609</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>4804</v>
+        <v>4789</v>
       </c>
       <c r="F47" s="3" t="s">
-        <v>4786</v>
+        <v>4771</v>
       </c>
       <c r="G47" s="3">
         <v>3.5301999999999998</v>
@@ -78682,16 +78804,16 @@
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A48" s="10" t="s">
-        <v>4586</v>
+        <v>4571</v>
       </c>
       <c r="B48" s="10" t="s">
-        <v>4625</v>
+        <v>4610</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>4805</v>
+        <v>4790</v>
       </c>
       <c r="F48" s="3" t="s">
-        <v>4792</v>
+        <v>4777</v>
       </c>
       <c r="G48" s="3">
         <v>9.4116</v>
@@ -78702,15 +78824,15 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" s="10" t="s">
-        <v>4587</v>
+        <v>4572</v>
       </c>
       <c r="B49" s="10" t="s">
-        <v>4626</v>
+        <v>4611</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" s="10" t="s">
-        <v>4588</v>
+        <v>4573</v>
       </c>
       <c r="B50" s="10" t="s">
         <v>2365</v>
@@ -78726,7 +78848,7 @@
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" s="10" t="s">
-        <v>4589</v>
+        <v>4574</v>
       </c>
       <c r="B52" s="10" t="s">
         <v>2377</v>
@@ -78734,7 +78856,7 @@
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" s="10" t="s">
-        <v>4590</v>
+        <v>4575</v>
       </c>
       <c r="B53" s="10" t="s">
         <v>3055</v>
@@ -78742,7 +78864,7 @@
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54" s="10" t="s">
-        <v>4591</v>
+        <v>4576</v>
       </c>
       <c r="B54" s="10" t="s">
         <v>3070</v>
@@ -78750,7 +78872,7 @@
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55" s="10" t="s">
-        <v>4592</v>
+        <v>4577</v>
       </c>
       <c r="B55" s="10" t="s">
         <v>4005</v>
@@ -78758,7 +78880,7 @@
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56" s="10" t="s">
-        <v>4593</v>
+        <v>4578</v>
       </c>
       <c r="B56" s="10" t="s">
         <v>3058</v>
@@ -78766,7 +78888,7 @@
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57" s="10" t="s">
-        <v>4594</v>
+        <v>4579</v>
       </c>
       <c r="B57" s="10" t="s">
         <v>2599</v>
@@ -78774,15 +78896,15 @@
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A58" s="10" t="s">
-        <v>4595</v>
+        <v>4580</v>
       </c>
       <c r="B58" s="10" t="s">
-        <v>4627</v>
+        <v>4612</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A59" s="10" t="s">
-        <v>4596</v>
+        <v>4581</v>
       </c>
       <c r="B59" s="10" t="s">
         <v>3061</v>
@@ -78790,15 +78912,15 @@
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A60" s="10" t="s">
-        <v>4597</v>
+        <v>4582</v>
       </c>
       <c r="B60" s="10" t="s">
-        <v>4628</v>
+        <v>4613</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A61" s="10" t="s">
-        <v>4598</v>
+        <v>4583</v>
       </c>
       <c r="B61" s="10" t="s">
         <v>3067</v>
@@ -78816,12 +78938,12 @@
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B64" s="10" t="s">
-        <v>4629</v>
+        <v>4614</v>
       </c>
     </row>
     <row r="65" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B65" s="10" t="s">
-        <v>4630</v>
+        <v>4615</v>
       </c>
     </row>
     <row r="66" spans="2:2" x14ac:dyDescent="0.3">
@@ -78851,7 +78973,7 @@
     </row>
     <row r="71" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B71" s="10" t="s">
-        <v>4631</v>
+        <v>4616</v>
       </c>
     </row>
     <row r="72" spans="2:2" x14ac:dyDescent="0.3">
@@ -78886,7 +79008,7 @@
     </row>
     <row r="78" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B78" s="10" t="s">
-        <v>4632</v>
+        <v>4617</v>
       </c>
     </row>
     <row r="79" spans="2:2" x14ac:dyDescent="0.3">
@@ -78921,12 +79043,12 @@
     </row>
     <row r="85" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B85" s="10" t="s">
-        <v>4633</v>
+        <v>4618</v>
       </c>
     </row>
     <row r="86" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B86" s="10" t="s">
-        <v>4634</v>
+        <v>4619</v>
       </c>
     </row>
     <row r="87" spans="2:2" x14ac:dyDescent="0.3">
@@ -78946,37 +79068,37 @@
     </row>
     <row r="90" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B90" s="10" t="s">
-        <v>4635</v>
+        <v>4620</v>
       </c>
     </row>
     <row r="91" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B91" s="10" t="s">
-        <v>4636</v>
+        <v>4621</v>
       </c>
     </row>
     <row r="92" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B92" s="10" t="s">
-        <v>4637</v>
+        <v>4622</v>
       </c>
     </row>
     <row r="93" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B93" s="10" t="s">
-        <v>4638</v>
+        <v>4623</v>
       </c>
     </row>
     <row r="94" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B94" s="10" t="s">
-        <v>4639</v>
+        <v>4624</v>
       </c>
     </row>
     <row r="95" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B95" s="10" t="s">
-        <v>4640</v>
+        <v>4625</v>
       </c>
     </row>
     <row r="96" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B96" s="10" t="s">
-        <v>4641</v>
+        <v>4626</v>
       </c>
     </row>
     <row r="97" spans="2:2" x14ac:dyDescent="0.3">
@@ -78986,32 +79108,32 @@
     </row>
     <row r="98" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B98" s="10" t="s">
-        <v>4642</v>
+        <v>4627</v>
       </c>
     </row>
     <row r="99" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B99" s="10" t="s">
-        <v>4643</v>
+        <v>4628</v>
       </c>
     </row>
     <row r="100" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B100" s="10" t="s">
-        <v>4644</v>
+        <v>4629</v>
       </c>
     </row>
     <row r="101" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B101" s="10" t="s">
-        <v>4645</v>
+        <v>4630</v>
       </c>
     </row>
     <row r="102" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B102" s="10" t="s">
-        <v>4646</v>
+        <v>4631</v>
       </c>
     </row>
     <row r="103" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B103" s="10" t="s">
-        <v>4647</v>
+        <v>4632</v>
       </c>
     </row>
     <row r="104" spans="2:2" x14ac:dyDescent="0.3">
@@ -79021,7 +79143,7 @@
     </row>
     <row r="105" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B105" s="10" t="s">
-        <v>4648</v>
+        <v>4633</v>
       </c>
     </row>
     <row r="106" spans="2:2" x14ac:dyDescent="0.3">
@@ -79031,7 +79153,7 @@
     </row>
     <row r="107" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B107" s="10" t="s">
-        <v>4649</v>
+        <v>4634</v>
       </c>
     </row>
     <row r="108" spans="2:2" x14ac:dyDescent="0.3">
@@ -79041,7 +79163,7 @@
     </row>
     <row r="109" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B109" s="10" t="s">
-        <v>4650</v>
+        <v>4635</v>
       </c>
     </row>
     <row r="110" spans="2:2" x14ac:dyDescent="0.3">
@@ -79051,92 +79173,92 @@
     </row>
     <row r="111" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B111" s="10" t="s">
-        <v>4651</v>
+        <v>4636</v>
       </c>
     </row>
     <row r="112" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B112" s="10" t="s">
-        <v>4652</v>
+        <v>4637</v>
       </c>
     </row>
     <row r="113" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B113" s="10" t="s">
-        <v>4653</v>
+        <v>4638</v>
       </c>
     </row>
     <row r="114" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B114" s="10" t="s">
-        <v>4654</v>
+        <v>4639</v>
       </c>
     </row>
     <row r="115" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B115" s="10" t="s">
-        <v>4655</v>
+        <v>4640</v>
       </c>
     </row>
     <row r="116" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B116" s="10" t="s">
-        <v>4656</v>
+        <v>4641</v>
       </c>
     </row>
     <row r="117" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B117" s="10" t="s">
-        <v>4657</v>
+        <v>4642</v>
       </c>
     </row>
     <row r="118" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B118" s="10" t="s">
-        <v>4658</v>
+        <v>4643</v>
       </c>
     </row>
     <row r="119" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B119" s="10" t="s">
-        <v>4659</v>
+        <v>4644</v>
       </c>
     </row>
     <row r="120" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B120" s="10" t="s">
-        <v>4660</v>
+        <v>4645</v>
       </c>
     </row>
     <row r="121" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B121" s="10" t="s">
-        <v>4661</v>
+        <v>4646</v>
       </c>
     </row>
     <row r="122" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B122" s="10" t="s">
-        <v>4662</v>
+        <v>4647</v>
       </c>
     </row>
     <row r="123" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B123" s="10" t="s">
-        <v>4663</v>
+        <v>4648</v>
       </c>
     </row>
     <row r="124" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B124" s="10" t="s">
-        <v>4664</v>
+        <v>4649</v>
       </c>
     </row>
     <row r="125" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B125" s="10" t="s">
-        <v>4665</v>
+        <v>4650</v>
       </c>
     </row>
     <row r="126" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B126" s="10" t="s">
-        <v>4666</v>
+        <v>4651</v>
       </c>
     </row>
     <row r="127" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B127" s="10" t="s">
-        <v>4667</v>
+        <v>4652</v>
       </c>
     </row>
     <row r="128" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B128" s="10" t="s">
-        <v>4668</v>
+        <v>4653</v>
       </c>
     </row>
     <row r="129" spans="2:2" x14ac:dyDescent="0.3">
@@ -79171,12 +79293,12 @@
     </row>
     <row r="135" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B135" s="10" t="s">
-        <v>4669</v>
+        <v>4654</v>
       </c>
     </row>
     <row r="136" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B136" s="10" t="s">
-        <v>4670</v>
+        <v>4655</v>
       </c>
     </row>
     <row r="137" spans="2:2" x14ac:dyDescent="0.3">
@@ -79191,17 +79313,17 @@
     </row>
     <row r="139" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B139" s="10" t="s">
-        <v>4671</v>
+        <v>4656</v>
       </c>
     </row>
     <row r="140" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B140" s="10" t="s">
-        <v>4672</v>
+        <v>4657</v>
       </c>
     </row>
     <row r="141" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B141" s="10" t="s">
-        <v>4673</v>
+        <v>4658</v>
       </c>
     </row>
     <row r="142" spans="2:2" x14ac:dyDescent="0.3">
@@ -79216,12 +79338,12 @@
     </row>
     <row r="144" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B144" s="10" t="s">
-        <v>4674</v>
+        <v>4659</v>
       </c>
     </row>
     <row r="145" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B145" s="10" t="s">
-        <v>4675</v>
+        <v>4660</v>
       </c>
     </row>
     <row r="146" spans="2:2" x14ac:dyDescent="0.3">
@@ -79241,12 +79363,12 @@
     </row>
     <row r="149" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B149" s="10" t="s">
-        <v>4676</v>
+        <v>4661</v>
       </c>
     </row>
     <row r="150" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B150" s="10" t="s">
-        <v>4677</v>
+        <v>4662</v>
       </c>
     </row>
   </sheetData>

</xml_diff>